<commit_message>
assign period to citi positions; filter 'T' rows for ib nav,positions
</commit_message>
<xml_diff>
--- a/tests/data/mapping.xlsx
+++ b/tests/data/mapping.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22202"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="398">
   <si>
     <t>Theorem</t>
   </si>
@@ -1210,17 +1213,21 @@
   </si>
   <si>
     <t>Settlement Location</t>
+  </si>
+  <si>
+    <t>account_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1228,7 +1235,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1258,7 +1271,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1316,7 +1329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1351,7 +1364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1528,7 +1541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1538,11 +1551,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
@@ -1550,7 +1563,7 @@
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
@@ -1564,7 +1577,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -1578,7 +1591,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -1592,7 +1605,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -1606,7 +1619,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -1620,7 +1633,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -1634,7 +1647,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -1648,7 +1661,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1662,7 +1675,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -1676,7 +1689,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -1690,7 +1703,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -1704,7 +1717,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -1718,7 +1731,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -1732,7 +1745,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1746,7 +1759,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -1760,7 +1773,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1774,7 +1787,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -1788,7 +1801,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1802,7 +1815,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -1816,7 +1829,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1830,7 +1843,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1844,7 +1857,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -1858,7 +1871,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1872,7 +1885,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -1886,7 +1899,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1900,7 +1913,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -1914,7 +1927,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1928,7 +1941,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -1942,7 +1955,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -1956,7 +1969,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1970,7 +1983,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -1984,7 +1997,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1998,7 +2011,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -2012,7 +2025,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -2026,7 +2039,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -2040,7 +2053,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2068,7 +2081,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2082,7 +2095,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -2096,7 +2109,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2110,7 +2123,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2124,7 +2137,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2138,7 +2151,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2152,7 +2165,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2166,7 +2179,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2180,7 +2193,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2207,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2208,7 +2221,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -2222,7 +2235,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -2236,7 +2249,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -2250,7 +2263,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -2264,7 +2277,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -2278,7 +2291,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -2292,7 +2305,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -2306,7 +2319,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -2320,7 +2333,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -2334,7 +2347,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -2348,7 +2361,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2362,7 +2375,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -2376,7 +2389,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -2390,7 +2403,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -2404,7 +2417,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2418,7 +2431,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -2432,7 +2445,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2446,7 +2459,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -2460,7 +2473,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -2474,7 +2487,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -2488,7 +2501,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -2502,7 +2515,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -2516,7 +2529,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -2530,7 +2543,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -2544,7 +2557,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>141</v>
       </c>
@@ -2558,7 +2571,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2572,7 +2585,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -2586,7 +2599,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>144</v>
       </c>
@@ -2600,7 +2613,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -2614,7 +2627,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -2628,7 +2641,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -2642,7 +2655,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -2656,7 +2669,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -2670,7 +2683,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>150</v>
       </c>
@@ -2684,7 +2697,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -2698,7 +2711,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>141</v>
       </c>
@@ -2712,7 +2725,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>152</v>
       </c>
@@ -2726,7 +2739,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>153</v>
       </c>
@@ -2740,7 +2753,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>142</v>
       </c>
@@ -2754,7 +2767,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>154</v>
       </c>
@@ -2768,7 +2781,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -2782,7 +2795,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -2796,7 +2809,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>155</v>
       </c>
@@ -2810,7 +2823,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>156</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>157</v>
       </c>
@@ -2838,7 +2851,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>158</v>
       </c>
@@ -2852,7 +2865,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>159</v>
       </c>
@@ -2866,7 +2879,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>160</v>
       </c>
@@ -2880,7 +2893,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>161</v>
       </c>
@@ -2894,7 +2907,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>162</v>
       </c>
@@ -2908,7 +2921,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>163</v>
       </c>
@@ -2922,7 +2935,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>164</v>
       </c>
@@ -2936,7 +2949,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>165</v>
       </c>
@@ -2950,7 +2963,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>129</v>
       </c>
@@ -2964,7 +2977,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>198</v>
       </c>
@@ -2978,7 +2991,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>199</v>
       </c>
@@ -2992,7 +3005,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>140</v>
       </c>
@@ -3006,7 +3019,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>200</v>
       </c>
@@ -3020,7 +3033,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>201</v>
       </c>
@@ -3034,7 +3047,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>202</v>
       </c>
@@ -3048,7 +3061,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>203</v>
       </c>
@@ -3062,7 +3075,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>204</v>
       </c>
@@ -3076,7 +3089,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>205</v>
       </c>
@@ -3090,7 +3103,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>206</v>
       </c>
@@ -3104,7 +3117,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>145</v>
       </c>
@@ -3118,7 +3131,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>207</v>
       </c>
@@ -3132,7 +3145,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>208</v>
       </c>
@@ -3146,7 +3159,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>209</v>
       </c>
@@ -3160,7 +3173,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>210</v>
       </c>
@@ -3174,7 +3187,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>211</v>
       </c>
@@ -3188,7 +3201,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>159</v>
       </c>
@@ -3202,7 +3215,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>212</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>213</v>
       </c>
@@ -3230,7 +3243,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>214</v>
       </c>
@@ -3244,7 +3257,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>215</v>
       </c>
@@ -3258,7 +3271,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>216</v>
       </c>
@@ -3272,7 +3285,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>217</v>
       </c>
@@ -3286,7 +3299,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>218</v>
       </c>
@@ -3300,7 +3313,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>219</v>
       </c>
@@ -3314,7 +3327,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>220</v>
       </c>
@@ -3328,7 +3341,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>221</v>
       </c>
@@ -3342,7 +3355,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -3356,7 +3369,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>198</v>
       </c>
@@ -3370,7 +3383,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>206</v>
       </c>
@@ -3384,7 +3397,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>105</v>
       </c>
@@ -3398,7 +3411,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>238</v>
       </c>
@@ -3412,7 +3425,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>239</v>
       </c>
@@ -3426,7 +3439,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>240</v>
       </c>
@@ -3440,7 +3453,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -3454,7 +3467,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>242</v>
       </c>
@@ -3468,7 +3481,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>243</v>
       </c>
@@ -3482,7 +3495,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>244</v>
       </c>
@@ -3496,7 +3509,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>245</v>
       </c>
@@ -3510,7 +3523,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>246</v>
       </c>
@@ -3524,7 +3537,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>247</v>
       </c>
@@ -3538,7 +3551,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>248</v>
       </c>
@@ -3552,7 +3565,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>249</v>
       </c>
@@ -3566,7 +3579,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>250</v>
       </c>
@@ -3580,7 +3593,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>251</v>
       </c>
@@ -3594,7 +3607,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>129</v>
       </c>
@@ -3608,7 +3621,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>198</v>
       </c>
@@ -3622,7 +3635,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>205</v>
       </c>
@@ -3636,7 +3649,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>258</v>
       </c>
@@ -3650,7 +3663,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>259</v>
       </c>
@@ -3664,7 +3677,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>260</v>
       </c>
@@ -3678,7 +3691,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>261</v>
       </c>
@@ -3692,7 +3705,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>262</v>
       </c>
@@ -3706,7 +3719,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>263</v>
       </c>
@@ -3720,7 +3733,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>129</v>
       </c>
@@ -3734,7 +3747,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>198</v>
       </c>
@@ -3748,7 +3761,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>199</v>
       </c>
@@ -3762,7 +3775,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>140</v>
       </c>
@@ -3776,7 +3789,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>200</v>
       </c>
@@ -3790,7 +3803,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>201</v>
       </c>
@@ -3804,7 +3817,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>202</v>
       </c>
@@ -3818,7 +3831,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>203</v>
       </c>
@@ -3832,7 +3845,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>204</v>
       </c>
@@ -3846,7 +3859,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>205</v>
       </c>
@@ -3860,7 +3873,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>206</v>
       </c>
@@ -3874,7 +3887,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>139</v>
       </c>
@@ -3888,7 +3901,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>285</v>
       </c>
@@ -3902,7 +3915,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>286</v>
       </c>
@@ -3916,7 +3929,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>287</v>
       </c>
@@ -3930,7 +3943,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>145</v>
       </c>
@@ -3944,7 +3957,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>288</v>
       </c>
@@ -3958,7 +3971,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>289</v>
       </c>
@@ -3972,7 +3985,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>290</v>
       </c>
@@ -3986,7 +3999,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
         <v>291</v>
       </c>
@@ -4000,7 +4013,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
         <v>292</v>
       </c>
@@ -4014,7 +4027,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4">
       <c r="A177" t="s">
         <v>293</v>
       </c>
@@ -4028,7 +4041,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4">
       <c r="A178" t="s">
         <v>294</v>
       </c>
@@ -4042,7 +4055,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4">
       <c r="A179" t="s">
         <v>295</v>
       </c>
@@ -4056,7 +4069,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4">
       <c r="A180" t="s">
         <v>296</v>
       </c>
@@ -4070,7 +4083,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4">
       <c r="A181" t="s">
         <v>142</v>
       </c>
@@ -4084,7 +4097,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4">
       <c r="A182" t="s">
         <v>214</v>
       </c>
@@ -4098,7 +4111,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4">
       <c r="A183" t="s">
         <v>297</v>
       </c>
@@ -4112,7 +4125,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4">
       <c r="A184" t="s">
         <v>298</v>
       </c>
@@ -4126,7 +4139,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4">
       <c r="A185" t="s">
         <v>299</v>
       </c>
@@ -4140,7 +4153,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4">
       <c r="A186" t="s">
         <v>218</v>
       </c>
@@ -4154,7 +4167,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187" t="s">
         <v>219</v>
       </c>
@@ -4168,7 +4181,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188" t="s">
         <v>300</v>
       </c>
@@ -4182,7 +4195,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="A189" t="s">
         <v>301</v>
       </c>
@@ -4196,7 +4209,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="A190" t="s">
         <v>152</v>
       </c>
@@ -4210,7 +4223,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="A191" t="s">
         <v>144</v>
       </c>
@@ -4224,7 +4237,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4">
       <c r="A192" t="s">
         <v>302</v>
       </c>
@@ -4238,7 +4251,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4">
       <c r="A193" t="s">
         <v>303</v>
       </c>
@@ -4252,7 +4265,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4">
       <c r="A194" t="s">
         <v>304</v>
       </c>
@@ -4266,7 +4279,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>305</v>
       </c>
@@ -4280,7 +4293,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>306</v>
       </c>
@@ -4294,7 +4307,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>307</v>
       </c>
@@ -4308,7 +4321,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4">
       <c r="A198" t="s">
         <v>308</v>
       </c>
@@ -4322,7 +4335,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
         <v>145</v>
       </c>
@@ -4336,7 +4349,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4">
       <c r="A200" t="s">
         <v>216</v>
       </c>
@@ -4350,7 +4363,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4">
       <c r="A201" t="s">
         <v>205</v>
       </c>
@@ -4364,7 +4377,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4">
       <c r="A202" t="s">
         <v>309</v>
       </c>
@@ -4378,7 +4391,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4">
       <c r="A203" t="s">
         <v>139</v>
       </c>
@@ -4392,7 +4405,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4">
       <c r="A204" t="s">
         <v>310</v>
       </c>
@@ -4406,7 +4419,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4">
       <c r="A205" t="s">
         <v>198</v>
       </c>
@@ -4420,7 +4433,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4">
       <c r="A206" t="s">
         <v>311</v>
       </c>
@@ -4434,7 +4447,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4">
       <c r="A207" t="s">
         <v>305</v>
       </c>
@@ -4448,7 +4461,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4">
       <c r="A208" t="s">
         <v>306</v>
       </c>
@@ -4462,7 +4475,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4">
       <c r="A209" t="s">
         <v>308</v>
       </c>
@@ -4476,7 +4489,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4">
       <c r="A210" t="s">
         <v>312</v>
       </c>
@@ -4490,7 +4503,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4">
       <c r="A211" t="s">
         <v>216</v>
       </c>
@@ -4504,7 +4517,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4">
       <c r="A212" t="s">
         <v>313</v>
       </c>
@@ -4518,7 +4531,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4">
       <c r="A213" t="s">
         <v>314</v>
       </c>
@@ -4532,7 +4545,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4">
       <c r="A214" t="s">
         <v>315</v>
       </c>
@@ -4546,7 +4559,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4">
       <c r="A215" t="s">
         <v>307</v>
       </c>
@@ -4560,9 +4573,9 @@
         <v>329</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
       <c r="B216" t="s">
         <v>337</v>
@@ -4574,7 +4587,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4">
       <c r="A217" t="s">
         <v>316</v>
       </c>
@@ -4588,7 +4601,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4">
       <c r="A218" t="s">
         <v>317</v>
       </c>
@@ -4602,7 +4615,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4">
       <c r="A219" t="s">
         <v>153</v>
       </c>
@@ -4616,7 +4629,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4">
       <c r="A220" t="s">
         <v>308</v>
       </c>
@@ -4630,7 +4643,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4">
       <c r="A221" t="s">
         <v>307</v>
       </c>
@@ -4644,7 +4657,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4">
       <c r="A222" t="s">
         <v>318</v>
       </c>
@@ -4658,7 +4671,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4">
       <c r="A223" t="s">
         <v>319</v>
       </c>
@@ -4672,7 +4685,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4">
       <c r="A224" t="s">
         <v>320</v>
       </c>
@@ -4686,7 +4699,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4">
       <c r="A225" t="s">
         <v>321</v>
       </c>
@@ -4700,7 +4713,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>322</v>
       </c>
@@ -4714,7 +4727,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4">
       <c r="A227" t="s">
         <v>323</v>
       </c>
@@ -4728,7 +4741,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4">
       <c r="A228" t="s">
         <v>324</v>
       </c>
@@ -4742,7 +4755,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4">
       <c r="A229" t="s">
         <v>325</v>
       </c>
@@ -4756,7 +4769,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4">
       <c r="A230" t="s">
         <v>326</v>
       </c>
@@ -4770,7 +4783,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>198</v>
       </c>
@@ -4784,7 +4797,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4">
       <c r="A232" t="s">
         <v>139</v>
       </c>
@@ -4798,7 +4811,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4">
       <c r="A233" t="s">
         <v>144</v>
       </c>
@@ -4812,7 +4825,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4">
       <c r="A234" t="s">
         <v>303</v>
       </c>
@@ -4826,7 +4839,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4">
       <c r="A235" t="s">
         <v>287</v>
       </c>
@@ -4840,7 +4853,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4">
       <c r="A236" t="s">
         <v>305</v>
       </c>
@@ -4854,7 +4867,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4">
       <c r="A237" t="s">
         <v>306</v>
       </c>
@@ -4868,7 +4881,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>307</v>
       </c>
@@ -4882,7 +4895,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4">
       <c r="A239" t="s">
         <v>308</v>
       </c>
@@ -4896,7 +4909,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>145</v>
       </c>
@@ -4910,7 +4923,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4">
       <c r="A241" t="s">
         <v>216</v>
       </c>
@@ -4924,7 +4937,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4">
       <c r="A242" t="s">
         <v>205</v>
       </c>
@@ -4938,7 +4951,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4">
       <c r="A243" t="s">
         <v>331</v>
       </c>
@@ -4952,7 +4965,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4">
       <c r="A244" t="s">
         <v>332</v>
       </c>
@@ -4966,7 +4979,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4">
       <c r="A245" t="s">
         <v>333</v>
       </c>
@@ -4980,7 +4993,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4">
       <c r="A246" t="s">
         <v>334</v>
       </c>
@@ -4994,7 +5007,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4">
       <c r="A247" t="s">
         <v>335</v>
       </c>
@@ -5009,7 +5022,13 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix pershing position empty field issues
</commit_message>
<xml_diff>
--- a/tests/data/mapping.xlsx
+++ b/tests/data/mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22202"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16940" yWindow="7400" windowWidth="22260" windowHeight="12640"/>
+    <workbookView xWindow="8500" yWindow="3140" windowWidth="25600" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="409">
   <si>
     <t>Theorem</t>
   </si>
@@ -1223,13 +1223,48 @@
   </si>
   <si>
     <t>citi_positions_valuations</t>
+  </si>
+  <si>
+    <t>CUSIP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pershing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pershing_positions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>coupon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coupon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effective Maturity Date</t>
+  </si>
+  <si>
+    <t>maturity_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1267,13 +1302,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1285,23 +1331,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1571,7 +1622,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1579,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D258"/>
+  <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="B248" sqref="B248"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2746,7 +2797,7 @@
         <v>141</v>
       </c>
       <c r="B83" t="s">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="C83" t="s">
         <v>195</v>
@@ -2757,10 +2808,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C84" t="s">
         <v>195</v>
@@ -2771,10 +2822,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C85" t="s">
         <v>195</v>
@@ -2785,10 +2836,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
-        <v>278</v>
+        <v>370</v>
       </c>
       <c r="C86" t="s">
         <v>195</v>
@@ -2799,10 +2850,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B87" t="s">
-        <v>371</v>
+        <v>278</v>
       </c>
       <c r="C87" t="s">
         <v>195</v>
@@ -2813,10 +2864,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B88" t="s">
-        <v>178</v>
+        <v>371</v>
       </c>
       <c r="C88" t="s">
         <v>195</v>
@@ -2827,10 +2878,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B89" t="s">
-        <v>372</v>
+        <v>178</v>
       </c>
       <c r="C89" t="s">
         <v>195</v>
@@ -2841,10 +2892,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B90" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C90" t="s">
         <v>195</v>
@@ -2855,10 +2906,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B91" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C91" t="s">
         <v>195</v>
@@ -2869,10 +2920,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B92" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C92" t="s">
         <v>195</v>
@@ -2883,10 +2934,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B93" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C93" t="s">
         <v>195</v>
@@ -2897,10 +2948,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B94" t="s">
-        <v>346</v>
+        <v>376</v>
       </c>
       <c r="C94" t="s">
         <v>195</v>
@@ -2911,10 +2962,10 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B95" t="s">
-        <v>377</v>
+        <v>346</v>
       </c>
       <c r="C95" t="s">
         <v>195</v>
@@ -2925,10 +2976,10 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B96" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C96" t="s">
         <v>195</v>
@@ -2939,10 +2990,10 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B97" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C97" t="s">
         <v>195</v>
@@ -2953,10 +3004,10 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B98" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C98" t="s">
         <v>195</v>
@@ -2967,10 +3018,10 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B99" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C99" t="s">
         <v>195</v>
@@ -2981,10 +3032,10 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C100" t="s">
         <v>195</v>
@@ -2995,66 +3046,66 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>129</v>
+        <v>401</v>
       </c>
       <c r="B101" t="s">
-        <v>167</v>
+        <v>402</v>
       </c>
       <c r="C101" t="s">
-        <v>196</v>
+        <v>403</v>
       </c>
       <c r="D101" t="s">
-        <v>197</v>
+        <v>404</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>198</v>
+        <v>405</v>
       </c>
       <c r="B102" t="s">
-        <v>168</v>
+        <v>406</v>
       </c>
       <c r="C102" t="s">
-        <v>196</v>
+        <v>403</v>
       </c>
       <c r="D102" t="s">
-        <v>197</v>
+        <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>199</v>
-      </c>
-      <c r="B103" t="s">
-        <v>169</v>
+        <v>408</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>407</v>
       </c>
       <c r="C103" t="s">
-        <v>196</v>
+        <v>403</v>
       </c>
       <c r="D103" t="s">
-        <v>197</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
+        <v>382</v>
       </c>
       <c r="C104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="B105" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C105" t="s">
         <v>196</v>
@@ -3065,10 +3116,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B106" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C106" t="s">
         <v>196</v>
@@ -3079,10 +3130,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B107" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C107" t="s">
         <v>196</v>
@@ -3093,10 +3144,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>203</v>
+        <v>140</v>
       </c>
       <c r="B108" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C108" t="s">
         <v>196</v>
@@ -3107,10 +3158,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B109" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C109" t="s">
         <v>196</v>
@@ -3121,10 +3172,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B110" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C110" t="s">
         <v>196</v>
@@ -3135,10 +3186,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B111" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C111" t="s">
         <v>196</v>
@@ -3149,10 +3200,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="B112" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C112" t="s">
         <v>196</v>
@@ -3163,10 +3214,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B113" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C113" t="s">
         <v>196</v>
@@ -3177,10 +3228,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B114" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C114" t="s">
         <v>196</v>
@@ -3191,10 +3242,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B115" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C115" t="s">
         <v>196</v>
@@ -3205,10 +3256,10 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>145</v>
       </c>
       <c r="B116" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C116" t="s">
         <v>196</v>
@@ -3219,10 +3270,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B117" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C117" t="s">
         <v>196</v>
@@ -3233,10 +3284,10 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="B118" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C118" t="s">
         <v>196</v>
@@ -3247,10 +3298,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B119" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C119" t="s">
         <v>196</v>
@@ -3261,10 +3312,10 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B120" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C120" t="s">
         <v>196</v>
@@ -3275,10 +3326,10 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B121" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C121" t="s">
         <v>196</v>
@@ -3289,10 +3340,10 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>215</v>
+        <v>159</v>
       </c>
       <c r="B122" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C122" t="s">
         <v>196</v>
@@ -3303,10 +3354,10 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B123" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C123" t="s">
         <v>196</v>
@@ -3317,10 +3368,10 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B124" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C124" t="s">
         <v>196</v>
@@ -3331,10 +3382,10 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B125" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C125" t="s">
         <v>196</v>
@@ -3345,10 +3396,10 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B126" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C126" t="s">
         <v>196</v>
@@ -3359,10 +3410,10 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B127" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C127" t="s">
         <v>196</v>
@@ -3373,10 +3424,10 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B128" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C128" t="s">
         <v>196</v>
@@ -3387,66 +3438,66 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>218</v>
       </c>
       <c r="B129" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="C129" t="s">
         <v>196</v>
       </c>
       <c r="D129" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="B130" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="C130" t="s">
         <v>196</v>
       </c>
       <c r="D130" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B131" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="C131" t="s">
         <v>196</v>
       </c>
       <c r="D131" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>105</v>
+        <v>221</v>
       </c>
       <c r="B132" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="C132" t="s">
         <v>196</v>
       </c>
       <c r="D132" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>238</v>
+        <v>129</v>
       </c>
       <c r="B133" t="s">
-        <v>223</v>
+        <v>167</v>
       </c>
       <c r="C133" t="s">
         <v>196</v>
@@ -3457,10 +3508,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="B134" t="s">
-        <v>224</v>
+        <v>168</v>
       </c>
       <c r="C134" t="s">
         <v>196</v>
@@ -3471,10 +3522,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="B135" t="s">
-        <v>225</v>
+        <v>177</v>
       </c>
       <c r="C135" t="s">
         <v>196</v>
@@ -3485,10 +3536,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>241</v>
+        <v>105</v>
       </c>
       <c r="B136" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C136" t="s">
         <v>196</v>
@@ -3499,10 +3550,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B137" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C137" t="s">
         <v>196</v>
@@ -3513,10 +3564,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B138" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C138" t="s">
         <v>196</v>
@@ -3527,10 +3578,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B139" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C139" t="s">
         <v>196</v>
@@ -3541,10 +3592,10 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B140" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C140" t="s">
         <v>196</v>
@@ -3555,10 +3606,10 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B141" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C141" t="s">
         <v>196</v>
@@ -3569,10 +3620,10 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B142" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C142" t="s">
         <v>196</v>
@@ -3583,10 +3634,10 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B143" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C143" t="s">
         <v>196</v>
@@ -3597,10 +3648,10 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B144" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C144" t="s">
         <v>196</v>
@@ -3611,10 +3662,10 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B145" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C145" t="s">
         <v>196</v>
@@ -3625,10 +3676,10 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B146" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C146" t="s">
         <v>196</v>
@@ -3639,66 +3690,66 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>129</v>
+        <v>248</v>
       </c>
       <c r="B147" t="s">
-        <v>167</v>
+        <v>233</v>
       </c>
       <c r="C147" t="s">
         <v>196</v>
       </c>
       <c r="D147" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
       <c r="B148" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="C148" t="s">
         <v>196</v>
       </c>
       <c r="D148" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="B149" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="C149" t="s">
         <v>196</v>
       </c>
       <c r="D149" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B150" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="C150" t="s">
         <v>196</v>
       </c>
       <c r="D150" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>259</v>
+        <v>129</v>
       </c>
       <c r="B151" t="s">
-        <v>253</v>
+        <v>167</v>
       </c>
       <c r="C151" t="s">
         <v>196</v>
@@ -3709,10 +3760,10 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>260</v>
+        <v>198</v>
       </c>
       <c r="B152" t="s">
-        <v>254</v>
+        <v>168</v>
       </c>
       <c r="C152" t="s">
         <v>196</v>
@@ -3723,10 +3774,10 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>261</v>
+        <v>205</v>
       </c>
       <c r="B153" t="s">
-        <v>255</v>
+        <v>176</v>
       </c>
       <c r="C153" t="s">
         <v>196</v>
@@ -3737,10 +3788,10 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B154" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C154" t="s">
         <v>196</v>
@@ -3751,10 +3802,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B155" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C155" t="s">
         <v>196</v>
@@ -3765,66 +3816,66 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>129</v>
+        <v>260</v>
       </c>
       <c r="B156" t="s">
-        <v>167</v>
+        <v>254</v>
       </c>
       <c r="C156" t="s">
         <v>196</v>
       </c>
       <c r="D156" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>198</v>
+        <v>261</v>
       </c>
       <c r="B157" t="s">
-        <v>168</v>
+        <v>255</v>
       </c>
       <c r="C157" t="s">
         <v>196</v>
       </c>
       <c r="D157" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>199</v>
+        <v>262</v>
       </c>
       <c r="B158" t="s">
-        <v>169</v>
+        <v>256</v>
       </c>
       <c r="C158" t="s">
         <v>196</v>
       </c>
       <c r="D158" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>140</v>
+        <v>263</v>
       </c>
       <c r="B159" t="s">
-        <v>170</v>
+        <v>257</v>
       </c>
       <c r="C159" t="s">
         <v>196</v>
       </c>
       <c r="D159" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="B160" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C160" t="s">
         <v>196</v>
@@ -3835,10 +3886,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B161" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C161" t="s">
         <v>196</v>
@@ -3849,10 +3900,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B162" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C162" t="s">
         <v>196</v>
@@ -3863,10 +3914,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>203</v>
+        <v>140</v>
       </c>
       <c r="B163" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C163" t="s">
         <v>196</v>
@@ -3877,10 +3928,10 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B164" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C164" t="s">
         <v>196</v>
@@ -3891,10 +3942,10 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B165" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C165" t="s">
         <v>196</v>
@@ -3905,10 +3956,10 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B166" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C166" t="s">
         <v>196</v>
@@ -3919,10 +3970,10 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="B167" t="s">
-        <v>265</v>
+        <v>174</v>
       </c>
       <c r="C167" t="s">
         <v>196</v>
@@ -3933,10 +3984,10 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>285</v>
+        <v>204</v>
       </c>
       <c r="B168" t="s">
-        <v>266</v>
+        <v>175</v>
       </c>
       <c r="C168" t="s">
         <v>196</v>
@@ -3947,10 +3998,10 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>286</v>
+        <v>205</v>
       </c>
       <c r="B169" t="s">
-        <v>267</v>
+        <v>176</v>
       </c>
       <c r="C169" t="s">
         <v>196</v>
@@ -3961,10 +4012,10 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>287</v>
+        <v>206</v>
       </c>
       <c r="B170" t="s">
-        <v>268</v>
+        <v>177</v>
       </c>
       <c r="C170" t="s">
         <v>196</v>
@@ -3975,10 +4026,10 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B171" t="s">
-        <v>178</v>
+        <v>265</v>
       </c>
       <c r="C171" t="s">
         <v>196</v>
@@ -3989,10 +4040,10 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B172" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C172" t="s">
         <v>196</v>
@@ -4003,10 +4054,10 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B173" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C173" t="s">
         <v>196</v>
@@ -4017,10 +4068,10 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B174" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C174" t="s">
         <v>196</v>
@@ -4031,10 +4082,10 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>291</v>
+        <v>145</v>
       </c>
       <c r="B175" t="s">
-        <v>272</v>
+        <v>178</v>
       </c>
       <c r="C175" t="s">
         <v>196</v>
@@ -4045,10 +4096,10 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B176" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C176" t="s">
         <v>196</v>
@@ -4059,10 +4110,10 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B177" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C177" t="s">
         <v>196</v>
@@ -4073,10 +4124,10 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B178" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C178" t="s">
         <v>196</v>
@@ -4087,10 +4138,10 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B179" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C179" t="s">
         <v>196</v>
@@ -4101,10 +4152,10 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B180" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C180" t="s">
         <v>196</v>
@@ -4115,10 +4166,10 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>142</v>
+        <v>293</v>
       </c>
       <c r="B181" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C181" t="s">
         <v>196</v>
@@ -4129,10 +4180,10 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>214</v>
+        <v>294</v>
       </c>
       <c r="B182" t="s">
-        <v>187</v>
+        <v>275</v>
       </c>
       <c r="C182" t="s">
         <v>196</v>
@@ -4143,10 +4194,10 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B183" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C183" t="s">
         <v>196</v>
@@ -4157,10 +4208,10 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B184" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C184" t="s">
         <v>196</v>
@@ -4171,10 +4222,10 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>299</v>
+        <v>142</v>
       </c>
       <c r="B185" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C185" t="s">
         <v>196</v>
@@ -4185,10 +4236,10 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B186" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C186" t="s">
         <v>196</v>
@@ -4199,10 +4250,10 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>219</v>
+        <v>297</v>
       </c>
       <c r="B187" t="s">
-        <v>192</v>
+        <v>279</v>
       </c>
       <c r="C187" t="s">
         <v>196</v>
@@ -4213,10 +4264,10 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B188" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C188" t="s">
         <v>196</v>
@@ -4227,10 +4278,10 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B189" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C189" t="s">
         <v>196</v>
@@ -4241,66 +4292,66 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
       <c r="B190" t="s">
-        <v>337</v>
+        <v>191</v>
       </c>
       <c r="C190" t="s">
-        <v>327</v>
+        <v>196</v>
       </c>
       <c r="D190" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="B191" t="s">
-        <v>359</v>
+        <v>192</v>
       </c>
       <c r="C191" t="s">
-        <v>327</v>
+        <v>196</v>
       </c>
       <c r="D191" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B192" t="s">
-        <v>360</v>
+        <v>282</v>
       </c>
       <c r="C192" t="s">
-        <v>327</v>
+        <v>196</v>
       </c>
       <c r="D192" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B193" t="s">
-        <v>361</v>
+        <v>283</v>
       </c>
       <c r="C193" t="s">
-        <v>327</v>
+        <v>196</v>
       </c>
       <c r="D193" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>304</v>
+        <v>152</v>
       </c>
       <c r="B194" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="C194" t="s">
         <v>327</v>
@@ -4311,10 +4362,10 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>305</v>
+        <v>144</v>
       </c>
       <c r="B195" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
       <c r="C195" t="s">
         <v>327</v>
@@ -4325,10 +4376,10 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B196" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="C196" t="s">
         <v>327</v>
@@ -4339,10 +4390,10 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B197" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="C197" t="s">
         <v>327</v>
@@ -4353,10 +4404,10 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B198" t="s">
-        <v>341</v>
+        <v>362</v>
       </c>
       <c r="C198" t="s">
         <v>327</v>
@@ -4367,10 +4418,10 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>145</v>
+        <v>305</v>
       </c>
       <c r="B199" t="s">
-        <v>178</v>
+        <v>343</v>
       </c>
       <c r="C199" t="s">
         <v>327</v>
@@ -4381,10 +4432,10 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>216</v>
+        <v>306</v>
       </c>
       <c r="B200" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C200" t="s">
         <v>327</v>
@@ -4395,10 +4446,10 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>205</v>
+        <v>307</v>
       </c>
       <c r="B201" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C201" t="s">
         <v>327</v>
@@ -4409,10 +4460,10 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B202" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="C202" t="s">
         <v>327</v>
@@ -4423,10 +4474,10 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B203" t="s">
-        <v>365</v>
+        <v>178</v>
       </c>
       <c r="C203" t="s">
         <v>327</v>
@@ -4437,10 +4488,10 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>310</v>
+        <v>216</v>
       </c>
       <c r="B204" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="C204" t="s">
         <v>327</v>
@@ -4451,66 +4502,66 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B205" t="s">
-        <v>337</v>
+        <v>363</v>
       </c>
       <c r="C205" t="s">
         <v>327</v>
       </c>
       <c r="D205" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B206" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="C206" t="s">
         <v>327</v>
       </c>
       <c r="D206" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>305</v>
+        <v>139</v>
       </c>
       <c r="B207" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="C207" t="s">
         <v>327</v>
       </c>
       <c r="D207" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B208" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="C208" t="s">
         <v>327</v>
       </c>
       <c r="D208" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>308</v>
+        <v>198</v>
       </c>
       <c r="B209" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C209" t="s">
         <v>327</v>
@@ -4521,10 +4572,10 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B210" t="s">
-        <v>393</v>
+        <v>342</v>
       </c>
       <c r="C210" t="s">
         <v>327</v>
@@ -4535,10 +4586,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>216</v>
+        <v>305</v>
       </c>
       <c r="B211" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C211" t="s">
         <v>327</v>
@@ -4549,10 +4600,10 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="B212" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C212" t="s">
         <v>327</v>
@@ -4563,10 +4614,10 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B213" t="s">
-        <v>394</v>
+        <v>341</v>
       </c>
       <c r="C213" t="s">
         <v>327</v>
@@ -4577,10 +4628,10 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B214" t="s">
-        <v>340</v>
+        <v>393</v>
       </c>
       <c r="C214" t="s">
         <v>327</v>
@@ -4591,10 +4642,10 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>307</v>
+        <v>216</v>
       </c>
       <c r="B215" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C215" t="s">
         <v>327</v>
@@ -4605,66 +4656,66 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>397</v>
+        <v>313</v>
       </c>
       <c r="B216" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C216" t="s">
         <v>327</v>
       </c>
       <c r="D216" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B217" t="s">
-        <v>349</v>
+        <v>394</v>
       </c>
       <c r="C217" t="s">
         <v>327</v>
       </c>
       <c r="D217" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B218" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C218" t="s">
         <v>327</v>
       </c>
       <c r="D218" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>153</v>
+        <v>307</v>
       </c>
       <c r="B219" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C219" t="s">
         <v>327</v>
       </c>
       <c r="D219" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>308</v>
+        <v>397</v>
       </c>
       <c r="B220" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C220" t="s">
         <v>327</v>
@@ -4675,10 +4726,10 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="B221" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C221" t="s">
         <v>327</v>
@@ -4689,10 +4740,10 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B222" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="C222" t="s">
         <v>327</v>
@@ -4703,10 +4754,10 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>319</v>
+        <v>153</v>
       </c>
       <c r="B223" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="C223" t="s">
         <v>327</v>
@@ -4717,10 +4768,10 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="B224" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="C224" t="s">
         <v>327</v>
@@ -4731,10 +4782,10 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="B225" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C225" t="s">
         <v>327</v>
@@ -4745,10 +4796,10 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B226" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C226" t="s">
         <v>327</v>
@@ -4759,10 +4810,10 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B227" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C227" t="s">
         <v>327</v>
@@ -4773,10 +4824,10 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B228" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C228" t="s">
         <v>327</v>
@@ -4787,10 +4838,10 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B229" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C229" t="s">
         <v>327</v>
@@ -4801,10 +4852,10 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B230" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C230" t="s">
         <v>327</v>
@@ -4815,66 +4866,66 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>198</v>
+        <v>323</v>
       </c>
       <c r="B231" t="s">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="C231" t="s">
         <v>327</v>
       </c>
       <c r="D231" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>139</v>
+        <v>324</v>
       </c>
       <c r="B232" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="C232" t="s">
         <v>327</v>
       </c>
       <c r="D232" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>144</v>
+        <v>325</v>
       </c>
       <c r="B233" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C233" t="s">
         <v>327</v>
       </c>
       <c r="D233" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="B234" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C234" t="s">
         <v>327</v>
       </c>
       <c r="D234" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>198</v>
       </c>
       <c r="B235" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="C235" t="s">
         <v>327</v>
@@ -4885,10 +4936,10 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>305</v>
+        <v>139</v>
       </c>
       <c r="B236" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="C236" t="s">
         <v>327</v>
@@ -4899,10 +4950,10 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>306</v>
+        <v>144</v>
       </c>
       <c r="B237" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="C237" t="s">
         <v>327</v>
@@ -4913,10 +4964,10 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B238" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="C238" t="s">
         <v>327</v>
@@ -4927,10 +4978,10 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="B239" t="s">
-        <v>341</v>
+        <v>360</v>
       </c>
       <c r="C239" t="s">
         <v>327</v>
@@ -4941,10 +4992,10 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>145</v>
+        <v>305</v>
       </c>
       <c r="B240" t="s">
-        <v>178</v>
+        <v>343</v>
       </c>
       <c r="C240" t="s">
         <v>327</v>
@@ -4955,10 +5006,10 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>216</v>
+        <v>306</v>
       </c>
       <c r="B241" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C241" t="s">
         <v>327</v>
@@ -4969,10 +5020,10 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>205</v>
+        <v>307</v>
       </c>
       <c r="B242" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C242" t="s">
         <v>327</v>
@@ -4983,10 +5034,10 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="B243" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="C243" t="s">
         <v>327</v>
@@ -4997,10 +5048,10 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="B244" t="s">
-        <v>395</v>
+        <v>178</v>
       </c>
       <c r="C244" t="s">
         <v>327</v>
@@ -5011,10 +5062,10 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>333</v>
+        <v>216</v>
       </c>
       <c r="B245" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="C245" t="s">
         <v>327</v>
@@ -5025,10 +5076,10 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>334</v>
+        <v>205</v>
       </c>
       <c r="B246" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="C246" t="s">
         <v>327</v>
@@ -5039,10 +5090,10 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B247" t="s">
-        <v>393</v>
+        <v>364</v>
       </c>
       <c r="C247" t="s">
         <v>327</v>
@@ -5053,66 +5104,66 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>198</v>
+        <v>332</v>
       </c>
       <c r="B248" t="s">
-        <v>337</v>
+        <v>395</v>
       </c>
       <c r="C248" t="s">
-        <v>398</v>
+        <v>327</v>
       </c>
       <c r="D248" t="s">
-        <v>399</v>
+        <v>336</v>
       </c>
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>153</v>
+        <v>333</v>
       </c>
       <c r="B249" t="s">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="C249" t="s">
-        <v>398</v>
+        <v>327</v>
       </c>
       <c r="D249" t="s">
-        <v>399</v>
+        <v>336</v>
       </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="B250" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="C250" t="s">
-        <v>398</v>
+        <v>327</v>
       </c>
       <c r="D250" t="s">
-        <v>399</v>
+        <v>336</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="B251" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="C251" t="s">
-        <v>398</v>
+        <v>327</v>
       </c>
       <c r="D251" t="s">
-        <v>399</v>
+        <v>336</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>311</v>
+        <v>198</v>
       </c>
       <c r="B252" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C252" t="s">
         <v>398</v>
@@ -5123,10 +5174,10 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>305</v>
+        <v>153</v>
       </c>
       <c r="B253" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C253" t="s">
         <v>398</v>
@@ -5137,10 +5188,10 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="B254" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C254" t="s">
         <v>398</v>
@@ -5151,10 +5202,10 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>216</v>
+        <v>308</v>
       </c>
       <c r="B255" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C255" t="s">
         <v>398</v>
@@ -5165,10 +5216,10 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>159</v>
+        <v>311</v>
       </c>
       <c r="B256" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C256" t="s">
         <v>398</v>
@@ -5179,10 +5230,10 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B257" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C257" t="s">
         <v>398</v>
@@ -5193,15 +5244,71 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B258" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C258" t="s">
         <v>398</v>
       </c>
       <c r="D258" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" t="s">
+        <v>216</v>
+      </c>
+      <c r="B259" t="s">
+        <v>345</v>
+      </c>
+      <c r="C259" t="s">
+        <v>398</v>
+      </c>
+      <c r="D259" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" t="s">
+        <v>159</v>
+      </c>
+      <c r="B260" t="s">
+        <v>346</v>
+      </c>
+      <c r="C260" t="s">
+        <v>398</v>
+      </c>
+      <c r="D260" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" t="s">
+        <v>313</v>
+      </c>
+      <c r="B261" t="s">
+        <v>347</v>
+      </c>
+      <c r="C261" t="s">
+        <v>398</v>
+      </c>
+      <c r="D261" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" t="s">
+        <v>307</v>
+      </c>
+      <c r="B262" t="s">
+        <v>348</v>
+      </c>
+      <c r="C262" t="s">
+        <v>398</v>
+      </c>
+      <c r="D262" t="s">
         <v>399</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added cash balance import logics
</commit_message>
<xml_diff>
--- a/tests/data/mapping.xlsx
+++ b/tests/data/mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="417">
   <si>
     <t>Theorem</t>
   </si>
@@ -1258,13 +1258,37 @@
   <si>
     <t>maturity_date</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>citi_cash_balances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period </t>
+  </si>
+  <si>
+    <t>opening_balance</t>
+  </si>
+  <si>
+    <t>Opening Balance</t>
+  </si>
+  <si>
+    <t>ledger_balance</t>
+  </si>
+  <si>
+    <t>Ledger Balance</t>
+  </si>
+  <si>
+    <t>available_balance</t>
+  </si>
+  <si>
+    <t>Available Balance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1307,6 +1331,14 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1331,7 +1363,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1339,20 +1371,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1622,7 +1659,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1630,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D262"/>
+  <dimension ref="A1:E269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5228,7 +5265,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="257" spans="1:4">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
         <v>305</v>
       </c>
@@ -5242,7 +5279,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>306</v>
       </c>
@@ -5256,7 +5293,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="259" spans="1:4">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>216</v>
       </c>
@@ -5270,7 +5307,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>159</v>
       </c>
@@ -5284,7 +5321,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>313</v>
       </c>
@@ -5298,7 +5335,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>307</v>
       </c>
@@ -5311,6 +5348,111 @@
       <c r="D262" t="s">
         <v>399</v>
       </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E263" s="3"/>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B264" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D264" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E264" s="3"/>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E265" s="3"/>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D266" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E266" s="3"/>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D267" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E267" s="3"/>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C268" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D268" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E268" s="3"/>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E269" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>